<commit_message>
modified and reruned a few notebooks
</commit_message>
<xml_diff>
--- a/services/project-compliance/notebooks/project-compliance-validation.xlsx
+++ b/services/project-compliance/notebooks/project-compliance-validation.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>To ensure the efficient use of energy in mining operations, several measures are in place. These include the decarbonisation of the electricity supply, which can be achieved through the integration of renewable energy sources into the national grid or the installation of on-site renewable energy systems. Additionally, the electrification of the mine vehicle fleet is being considered to reduce fuel consumption in mobile machinery. Regular servicing of vehicles and machinery is also mandated to maintain optimal fuel efficiency.</t>
+          <t>To ensure the efficient use of energy in mining operations, several measures are in place. These include the decarbonisation of the electricity supply, which can be achieved through the integration of renewable energy sources into the national grid or the installation of on-site renewable energy systems. Additionally, the electrification of the mine vehicle fleet is being considered to reduce fuel consumption in mobile machinery. Regular servicing of vehicles and machinery is also emphasized to maintain optimal fuel efficiency.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -526,8 +526,8 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Water usage is monitored and managed through several measures to ensure efficiency. The water level data is evaluated annually against model predictions, and the model is recalibrated if significant variations are observed. Boreholes on neighboring farms are monitored monthly for water levels, and the data is collated quarterly and analyzed annually. Additionally, a water balance for the operations is updated regularly to aid future groundwater modeling.
-Recycling and reusing water are integral parts of the water management system. Effluent from treatment plants is recycled to the process water pond. The process water pond receives water from tailings thickener overflows, storm water pond, rail load-out, and TSF return water. Filtered raw water is used for gland seal water, dust suppression, and flocculant make-up. This comprehensive approach ensures that water is used efficiently and sustainably within the mining operations.</t>
+          <t>Water usage is monitored and managed through several measures to ensure efficiency. The water level data is evaluated annually against model predictions, and the model is recalibrated if significant variations are observed. Boreholes on neighboring farms are monitored monthly for water levels, and the data is collated quarterly and analyzed annually. A water balance for the mining operations is updated regularly to aid future groundwater modeling and predictions.
+Recycling and reusing water are integral parts of the water management strategy. Effluent from treatment plants is recycled to the process water pond. The process water pond receives water from tailings thickener overflows, storm water pond, rail load-out, and TSF return water. Additionally, filtered raw water is used for gland seal water, dust suppression, and flocculant make-up. These measures ensure that water is reused efficiently within the mining operations.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -679,7 +679,8 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Steps being taken to optimize the use of raw materials and minimize waste include the decarbonisation of the electricity supply, electrification of the fleet, and regular servicing of vehicles and machinery to ensure optimal fuel efficiency. There is no benchmarking data available in the provided information to compare the mine's resource efficiency with industry standards.</t>
+          <t>To optimize the use of raw materials and minimize waste, several steps are being taken. These include promoting a culture of "conserve, reduce, reuse &amp; recycle" to minimize resource consumption and reduce potential waste. Additionally, domestic waste is sorted, with organic waste composted and cans and glass aggregated for recycling. Hazardous waste is removed by a licensed operator and disposed of at a registered hazardous waste facility.
+Regarding benchmarking data to compare the mine's resource efficiency with industry standards, there is no specific mention of such data being available. However, the implementation of these measures indicates a commitment to resource efficiency and waste minimization.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -746,7 +747,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Measures to monitor and control air emissions from mining activities include the regulation of all aspects of air quality through the National Environmental Management: Air Quality Act, which encompasses the prevention of pollution and environmental degradation, and the establishment of national norms and standards for air quality management. This includes air quality monitoring, management, and control, as well as the licensing of activities that result in atmospheric emissions. Additionally, the National Dust Control Regulations provide guidelines for monitoring and measuring dust fall, which is assessed for nuisance impact. Specific particulate matter monitoring involves setting up monitoring stations to measure PM10 and PM2.5 concentrations, as well as conducting dust fallout monitoring at sensitive receptor locations over specified periods.</t>
+          <t>Measures to monitor and control air emissions from mining activities include:
+1. **Particulate Matter Monitoring**: An ambient air quality monitoring survey for particulate matter and dust fallout was conducted, with a monitoring station set up approximately 2.6 km from the SE Pit. The survey provided data on PM10 and PM2.5 concentrations.
+2. **Dust Fallout Monitoring**: Dust fallout concentrations were monitored over two one-month periods at seven locations considered sensitive receptors, such as schools and homesteads around the South East Pit.
+3. **Vehicle Speed Control**: Reducing vehicle speeds to 40 km/hr on paved site roads and 20 km/hr on unpaved haul routes to minimize dust emissions.
+4. **Material Handling**: Utilizing chutes at material handling transfer points and ensuring vehicles carrying dry soil and other materials are covered during travel.
+5. **Surface Maintenance**: Maintaining the surface of haul routes with less erodible aggregate material.
+6. **Blasting Controls**: Implementing specific measures during blasting, such as monitoring air quality during the test phase, avoiding blasting during high wind speeds, and refraining from blasting during atmospheric inversion conditions or in fog.
+7. **Enclosed Processing Plant**: Ensuring the processing plant is enclosed and that all bag filters on extraction points are designed for 30 mg/Nm3.
+8. **Long-term Monitoring**: Conducting long-term air quality monitoring campaigns to ensure compliance with air quality standards.
+These measures aim to control and reduce emissions of particulate matter and other pollutants, ensuring compliance with relevant air quality standards and minimizing environmental impact.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -829,7 +839,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wastewater from mining operations is treated through a series of processes before being discharged. The raw water is pumped to a water treatment plant (WTP) where it undergoes direct flocculation filtration, UV sterilization, and chlorination to meet South African National Standards (SANS) and/or World Health Organization (WHO) standards. Effluent from these treatment plants, including regeneration and backwash, is recycled to the process water pond. Measures to prevent contamination of local water bodies include ensuring that clean and dirty water systems are kept separate and designed to handle specific storm events, preventing dirty water or substances that may cause pollution from entering clean water resources, and recycling water used in any process as far as practicable. Additionally, no residue or substance likely to cause pollution is used in the construction of any infrastructure that may cause water pollution.</t>
+          <t>Wastewater from mining operations is treated using a containerized wastewater treatment plant (WWTP) designed with the best available technology and within best practice guidelines. The clear water effluent from the WWTP is recycled back into the process water system. Additionally, measures to prevent contamination of local water bodies include storing chemicals and toxins in bunded areas, maintaining stormwater systems to prevent contaminated runoff, and ensuring all contaminated stormwater is conveyed to pollution control dams (PCDs) rather than being discharged into the natural environment. Regular monitoring and maintenance are conducted to ensure the effectiveness of these measures.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -930,8 +940,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>To prevent soil erosion and land degradation due to mining activities, several practices are in place. These include minimizing the infrastructure footprint, phased land clearance, concurrent rehabilitation, and implementing erosion controls if required. Additionally, there are measures to limit land use change to the infrastructure footprint and to rehabilitate by replacing topsoil at depths similar to pre-mining levels. 
-For land reclamation post-mining, the practices involve progressive rehabilitation of disturbed land to minimize the exposure of bare soils to erosive effects, and ensuring that soil resources are preserved for use in rehabilitation to support post-closure land capability.</t>
+          <t>To prevent soil erosion and land degradation due to mining activities, several practices are in place. These include:
+1. **Phased Land Clearance**: Clearing land in phases to minimize the area exposed to erosion at any given time.
+2. **Concurrent Rehabilitation**: Rehabilitating disturbed land progressively to reduce the duration that bare soils are exposed.
+3. **Erosion Controls**: Implementing erosion control measures such as silt fences, berms, and sandbags.
+4. **Demarcation of 'No-Go' Areas**: Designating specific areas where no activities are allowed to prevent soil compaction and erosion.
+5. **Revegetation**: Re-vegetating disturbed areas with indigenous grass to establish a protective cover and minimize soil erosion and dust emission.
+6. **Stockpile Management**: Limiting the height and slope of soil stockpiles, keeping them free of weeds, and ensuring they are not compacted.
+For land reclamation post-mining, the practices include:
+1. **Replacing Topsoil**: Rehabilitating by replacing topsoil at depths similar to pre-mining conditions.
+2. **Revegetation of Stockpiles**: Establishing vegetation cover on stockpiles to control erosion.
+3. **Concurrent Rehabilitation**: Conducting rehabilitation activities concurrently with mining operations to ensure timely restoration of land.
+4. **Post-Rehabilitation Audits**: Performing audits to assess the success of soil remediation and re-establishment of soil functionality, and implementing further measures if necessary.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1133,7 +1153,8 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hazardous waste generated by the mine is managed through a series of protocols designed to identify, store, and dispose of such waste safely. In the event of spills or accidental releases, the mine has specific emergency response procedures. These include notifying downstream residents and users, identifying and providing alternative resources if contamination impacts the environment, cutting off the source of the spill, containing the spill, pumping excess hazardous liquids into temporary containers for appropriate disposal, and removing hazardous substances from damaged infrastructure to a suitable storage area before repair or removal.</t>
+          <t>Hazardous waste generated by the mine is identified, stored, and disposed of through several protocols. Hazardous substances such as chemicals, fuel, and oils are stored in appropriate containment structures like industry-standard drip-trays or concrete bunded areas. Drip trays are used at fuel dispensing areas and beneath any standing machinery to prevent spills. Washing and cleaning of equipment are conducted in designated areas away from sensitive zones.
+In the event of spills or accidental releases, immediate cleanup is required, and contaminants are properly drained and disposed of using appropriate solid/hazardous waste facilities. Contaminated soil must be removed and rehabilitated promptly. Additionally, there are specific emergency response procedures for different scenarios, such as spillage of chemicals and discharge of dirty water, which include notifying relevant authorities, containing the spill, and taking measures to prevent further contamination.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1219,7 +1240,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The management of non-hazardous waste includes systems informed by national norms and standards for the storage of waste, as well as regulations for waste information and assessment for landfill disposal. These regulations have been taken into account in the project planning and assessment processes to ensure proper management and reduction of waste. Additionally, guidelines on the need and desirability of waste management have been considered as part of the project planning.</t>
+          <t>The management of non-hazardous waste includes several systems and initiatives. A culture of "conserve, reduce, reuse, and recycle" is promoted to minimize resource consumption and reduce potential waste. Adequate scavenger-proof rubbish bins and waste disposal facilities are provided on-site at strategic points in work areas, and workers are encouraged not to litter but to use these facilities. The bins are emptied regularly and the waste is taken to a registered landfill for disposal. Additionally, all general waste, construction-related plant, equipment, surplus rock, and other foreign materials are cleared and removed from the site.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">

</xml_diff>